<commit_message>
changes in output file name
</commit_message>
<xml_diff>
--- a/analysis_output.xlsx
+++ b/analysis_output.xlsx
@@ -421,19 +421,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>D:\Study\Evalix\Evalix\Converted\1-s2.0-S0306437924001698-main.txt</v>
+        <v>resume.txt</v>
       </c>
       <c r="B2">
-        <v>381</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>84</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>10510</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix:appending results in analysis Excel file
</commit_message>
<xml_diff>
--- a/analysis_output.xlsx
+++ b/analysis_output.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -421,24 +421,41 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>resume.txt</v>
+        <v>Two-Timescale Gradient Descent Ascent Algorithms for.txt</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>203</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>253</v>
+        <v>20425</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>A-computational-analysis-of-transcribed-speech-of-people_2025_Computer-Speec.txt</v>
+      </c>
+      <c r="B3">
+        <v>545</v>
+      </c>
+      <c r="C3">
+        <v>85</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>20501</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>